<commit_message>
Flagowanie mieszkan z work table, zaokraglanie cen, hiperlinki, wybranie kolumn w tabelach roboczych, dable przenoszone do inputu
</commit_message>
<xml_diff>
--- a/output/work_table_2.xlsx
+++ b/output/work_table_2.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA1"/>
+  <dimension ref="A1:P1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,127 +446,72 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Data wygaśnięcia</t>
+          <t>Link</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Link</t>
+          <t>Adres</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Link2</t>
+          <t>podzielnica</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Adres</t>
+          <t>Pośrednik?</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Dzielnica</t>
+          <t>Telefon</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>podzielnica</t>
+          <t>Cena</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Sprzedane?</t>
+          <t>Cena/m2</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Pośrednik?</t>
+          <t>m2</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Telefon</t>
+          <t>Pokoje</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>Cena</t>
+          <t>Piętro</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>Cena/m2</t>
+          <t>Rodzaj mieszkania</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>m2</t>
+          <t>Tabela dzwonienie</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>Pokoje</t>
+          <t>Max Cena Kupna</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>Piętro</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>Rodzaj mieszkania</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
           <t>Notatka</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>Tabela dzwonienie</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>m2_category</t>
-        </is>
-      </c>
-      <c r="U1" s="1" t="inlineStr">
-        <is>
-          <t>Cena/m2_mean_Dzielnica</t>
-        </is>
-      </c>
-      <c r="V1" s="1" t="inlineStr">
-        <is>
-          <t>maksymalna_cena_Dzielnica</t>
-        </is>
-      </c>
-      <c r="W1" s="1" t="inlineStr">
-        <is>
-          <t>additional_profit_Dzielnica</t>
-        </is>
-      </c>
-      <c r="X1" s="1" t="inlineStr">
-        <is>
-          <t>Cena/m2_mean_podzielnica</t>
-        </is>
-      </c>
-      <c r="Y1" s="1" t="inlineStr">
-        <is>
-          <t>maksymalna_cena_podzielnica</t>
-        </is>
-      </c>
-      <c r="Z1" s="1" t="inlineStr">
-        <is>
-          <t>additional_profit_podzielnica</t>
-        </is>
-      </c>
-      <c r="AA1" s="1" t="inlineStr">
-        <is>
-          <t>Duplicate</t>
         </is>
       </c>
     </row>

</xml_diff>